<commit_message>
xlsx, csv 파일 수정
</commit_message>
<xml_diff>
--- a/document/테이블명세.xlsx
+++ b/document/테이블명세.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\Tiget\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7484C3-63A5-45D9-9448-F79E94046F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CA53B1-B919-4E09-BBEC-77E9EF894EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="2790" windowWidth="25380" windowHeight="13200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="사용자정보" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="207">
   <si>
     <t>열 이름</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -844,6 +844,14 @@
   </si>
   <si>
     <t>delete_date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>가변문자열(225)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(225)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1804,7 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E862B38E-A4DF-4FD8-AAD4-089E98885ADD}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -12604,8 +12612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F95A67-83BB-4437-9E8C-769B804D26C5}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13389,13 +13397,13 @@
         <v>154</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>153</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>95</v>
@@ -13411,20 +13419,18 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>95</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="G8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -13435,18 +13441,20 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="G9" s="9"/>
+        <v>142</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -13458,13 +13466,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>143</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>142</v>
@@ -13483,16 +13491,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>95</v>
@@ -13508,13 +13516,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>145</v>
+        <v>64</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>142</v>
@@ -13532,11 +13540,11 @@
       <c r="B13" s="8">
         <v>8</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>

</xml_diff>